<commit_message>
deleted a few lines
</commit_message>
<xml_diff>
--- a/docs/establishments.xlsx
+++ b/docs/establishments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fernanda.dorea\Documents\GitHub\HSO\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C471060F-D1F7-41FB-AB5D-D2ACF273D36D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EC04EF-457A-4EF6-91CA-1F06DA93751F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="34995" windowHeight="18598" activeTab="1" xr2:uid="{BC9F9AC6-E6B5-4E26-8DC4-44951FDC5054}"/>
+    <workbookView xWindow="34669" yWindow="-109" windowWidth="23040" windowHeight="13898" activeTab="1" xr2:uid="{BC9F9AC6-E6B5-4E26-8DC4-44951FDC5054}"/>
   </bookViews>
   <sheets>
     <sheet name="instances" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="115">
   <si>
     <t>URI</t>
   </si>
@@ -205,42 +205,6 @@
     <t>Catering</t>
   </si>
   <si>
-    <t>E910A</t>
-  </si>
-  <si>
-    <t>Restaurant or Cafe or Pub or Bar or Hotel or Catering service</t>
-  </si>
-  <si>
-    <t>E920A</t>
-  </si>
-  <si>
-    <t>Mobile retailer or market/street vendor</t>
-  </si>
-  <si>
-    <t>E930A</t>
-  </si>
-  <si>
-    <t>Take-away or fast-food outlet</t>
-  </si>
-  <si>
-    <t>E940A</t>
-  </si>
-  <si>
-    <t>Canteen or workplace catering</t>
-  </si>
-  <si>
-    <t>E950A</t>
-  </si>
-  <si>
-    <t>Temporary mass catering (fairs or festivals)</t>
-  </si>
-  <si>
-    <t>E960A</t>
-  </si>
-  <si>
-    <t>Camp or picnic</t>
-  </si>
-  <si>
     <t>E983A</t>
   </si>
   <si>
@@ -407,24 +371,6 @@
   </si>
   <si>
     <t>HSO_0000048</t>
-  </si>
-  <si>
-    <t>HSO_0000049</t>
-  </si>
-  <si>
-    <t>HSO_0000050</t>
-  </si>
-  <si>
-    <t>HSO_0000051</t>
-  </si>
-  <si>
-    <t>HSO_0000052</t>
-  </si>
-  <si>
-    <t>HSO_0000053</t>
-  </si>
-  <si>
-    <t>HSO_0000054</t>
   </si>
   <si>
     <t>HSO_0000055</t>
@@ -846,30 +792,30 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -877,30 +823,30 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
@@ -908,13 +854,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
         <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
         <v>23</v>
@@ -922,30 +868,30 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D7" t="s">
         <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
         <v>27</v>
@@ -953,13 +899,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
         <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
         <v>31</v>
@@ -967,13 +913,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
         <v>33</v>
@@ -981,13 +927,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
         <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
         <v>35</v>
@@ -995,13 +941,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
         <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D12" t="s">
         <v>37</v>
@@ -1009,13 +955,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
         <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D13" t="s">
         <v>39</v>
@@ -1023,13 +969,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
         <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D14" t="s">
         <v>41</v>
@@ -1037,13 +983,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
         <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
         <v>43</v>
@@ -1051,13 +997,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
         <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D16" t="s">
         <v>45</v>
@@ -1065,13 +1011,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
         <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D17" t="s">
         <v>47</v>
@@ -1079,13 +1025,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
         <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D18" t="s">
         <v>49</v>
@@ -1093,30 +1039,30 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B19" t="s">
         <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
         <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B20" t="s">
         <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D20" t="s">
         <v>55</v>
@@ -1124,30 +1070,30 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D22" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1158,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54574A88-39BA-4139-88A7-51805D36031E}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1188,13 +1134,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -1202,13 +1148,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -1216,30 +1162,30 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>11</v>
@@ -1247,13 +1193,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>13</v>
@@ -1261,13 +1207,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>15</v>
@@ -1275,30 +1221,30 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>19</v>
@@ -1306,13 +1252,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>21</v>
@@ -1320,13 +1266,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>23</v>
@@ -1334,30 +1280,30 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>27</v>
@@ -1365,13 +1311,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>29</v>
@@ -1379,13 +1325,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>31</v>
@@ -1393,13 +1339,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>33</v>
@@ -1407,13 +1353,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>35</v>
@@ -1421,13 +1367,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>37</v>
@@ -1435,13 +1381,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>39</v>
@@ -1449,13 +1395,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>41</v>
@@ -1463,13 +1409,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>43</v>
@@ -1477,13 +1423,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>45</v>
@@ -1491,13 +1437,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>47</v>
@@ -1505,13 +1451,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>49</v>
@@ -1519,13 +1465,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B25" t="s">
         <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>51</v>
@@ -1533,145 +1479,61 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>53</v>
       </c>
       <c r="E26" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="A28" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B29" s="1" t="s">
+      <c r="A29" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" t="s">
-        <v>73</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" t="s">
-        <v>73</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" t="s">
-        <v>73</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" t="s">
-        <v>73</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" t="s">
-        <v>73</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>